<commit_message>
Updated car model drag coeff and added low drag configs
</commit_message>
<xml_diff>
--- a/OpenLap/SN3_120A.xlsx
+++ b/OpenLap/SN3_120A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Westo\OneDrive\Documents\GitHub\FEBSim\OpenLap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AEEE343-E108-46BA-BB03-F09AB59FCD36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5399DA4-F10E-437D-AD1E-CB2E0B47E8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1036,7 +1036,7 @@
   <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1161,7 +1161,7 @@
         <v>73</v>
       </c>
       <c r="C8" s="8">
-        <v>-2</v>
+        <v>-1.98</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>38</v>
@@ -1176,7 +1176,7 @@
         <v>74</v>
       </c>
       <c r="C9" s="3">
-        <v>-1.2</v>
+        <v>-1.33</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>38</v>
@@ -1217,7 +1217,8 @@
         <v>72</v>
       </c>
       <c r="C12" s="3">
-        <v>47</v>
+        <f>100-56.3</f>
+        <v>43.7</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>7</v>
@@ -1230,7 +1231,7 @@
         <v>17</v>
       </c>
       <c r="C13" s="3">
-        <v>1.1000000000000001</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>18</v>

</xml_diff>